<commit_message>
Updated code For Post Module in homescreen
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{92F48045-13AF-4745-A3B3-790064FB9067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BA217B9A-7BC2-4B30-ACE1-8A8289518B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
   </bookViews>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91130ACC-1138-46D1-A908-9CE5228C9D06}">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated code for create Post module in Company Page
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BA217B9A-7BC2-4B30-ACE1-8A8289518B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FD2C397E-8825-4417-9A0F-499076DDF1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
   </bookViews>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91130ACC-1138-46D1-A908-9CE5228C9D06}">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Completed script of all create post module
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FD2C397E-8825-4417-9A0F-499076DDF1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur More\eclipse-workspace\AndroidAppVersion2.0New\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08267D0C-B7FC-4311-8C4E-DA5F49ED620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -191,10 +195,6 @@
 YouTube - https://www.youtube.com/@ForttunaAwards
 Twitter - https://twitter.com/ForttunaAwards
 Facebook - https://www.facebook.com/forttunaaward?mibextid=LQQJ4d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The India hse summit &amp; Awards 2024 is a knowledge-based physical conference and the 7th edition of the flagship program hse summit by Synnex group. The 2-day summit strives to bring all key stakeholders—government officials, hse experts, industry associations and hse evangelists, technical leaders—together to discuss occupational safety and health &amp; EHS as a priority for companies while reiterating the significance and business benefits of investing in the health and safety of the workforce. This year the India hse summit &amp; awards 2024 is taking the initiative to spread awareness regarding the importance of occupational safety and health for the workforce in the ongoing covid19 pandemic with digitalization and technological solutions available to serve and save better</t>
   </si>
   <si>
     <t>ClubFees</t>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>2024 Production Testing  Awards event</t>
+  </si>
+  <si>
+    <t>The India hse summit &amp; Awards 2024 is a knowledge-based physical conference and the 7th edition of the flagship program hse summit by Synnex group. The 2-day summit strives to bring all key stakeholders—government officials, hse experts, industry associations and hse evangelists, technical leaders—together to discuss occupational safety and health &amp; EHS as a priority for companies while reiterating the significance and business benefits of investing in the health and safety of the workforce. This year the India hse summit &amp; awards 2024 is taking the initiative to spread awareness regarding the importance of occupational safety and health for the workforce in the ongoing covid19 pandemic with digitalization and technological solutions available to serve and save better</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,7 @@
   <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -825,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
@@ -836,25 +839,25 @@
         <v>8779549244</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>31</v>
@@ -911,7 +914,7 @@
         <v>37</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB2" s="4" t="s">
         <v>53</v>
@@ -921,10 +924,10 @@
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="AG2" s="2">
         <v>499</v>

</xml_diff>

<commit_message>
event module script completed
</commit_message>
<xml_diff>
--- a/TestData/Datasheet.xlsx
+++ b/TestData/Datasheet.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayur More\eclipse-workspace\AndroidAppVersion2.0New\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08267D0C-B7FC-4311-8C4E-DA5F49ED620A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D333CF95-CAEA-4166-943C-20CA8A6A790D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1E2BD0BB-FCCA-43DE-A424-1FEE5688881A}"/>
   </bookViews>
@@ -16,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,9 +177,6 @@
   </si>
   <si>
     <t>EventVenue</t>
-  </si>
-  <si>
-    <t>Vashi</t>
   </si>
   <si>
     <t>Deep learning enhances efficiency and accuracy in documenting repetitive testing activities. AI in software testing minimizes human error and enhances fault detection capabilities.</t>
@@ -267,6 +260,9 @@
   </si>
   <si>
     <t>The India hse summit &amp; Awards 2024 is a knowledge-based physical conference and the 7th edition of the flagship program hse summit by Synnex group. The 2-day summit strives to bring all key stakeholders—government officials, hse experts, industry associations and hse evangelists, technical leaders—together to discuss occupational safety and health &amp; EHS as a priority for companies while reiterating the significance and business benefits of investing in the health and safety of the workforce. This year the India hse summit &amp; awards 2024 is taking the initiative to spread awareness regarding the importance of occupational safety and health for the workforce in the ongoing covid19 pandemic with digitalization and technological solutions available to serve and save better</t>
+  </si>
+  <si>
+    <t>Vashi, Navi Mumbai</t>
   </si>
 </sst>
 </file>
@@ -702,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91130ACC-1138-46D1-A908-9CE5228C9D06}">
   <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
@@ -839,25 +835,25 @@
         <v>8779549244</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>31</v>
@@ -914,20 +910,20 @@
         <v>37</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AG2" s="2">
         <v>499</v>

</xml_diff>